<commit_message>
Updated version that allows users to register with a username, password, and email. It also displays the current schedule.
</commit_message>
<xml_diff>
--- a/updated_schedule.xlsx
+++ b/updated_schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +441,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Rank</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t xml:space="preserve">Saturday </t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Saturday </t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Monday</t>
         </is>
@@ -486,7 +481,11 @@
           <t>Pool Hours</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10:45-8</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>10:45-8</t>
@@ -499,25 +498,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10:45-8</t>
+          <t>10:45-9</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10:45-9</t>
+          <t>10:30-8</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10:30-8</t>
+          <t>11:00-8</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>11:00-8</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
         <is>
           <t>closed</t>
         </is>
@@ -525,38 +519,37 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>June18th</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>June18th</t>
+          <t>June19th</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>June19th</t>
+          <t>June20th</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>June20th</t>
+          <t>June21st</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>June21st</t>
+          <t>June22nd</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>June22nd</t>
+          <t>June23rd</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
-        <is>
-          <t>June23rd</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>June24th</t>
         </is>
@@ -568,8 +561,10 @@
           <t>Barry Ray</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -597,11 +592,6 @@
         </is>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -613,8 +603,10 @@
           <t>Blake Butz</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10:30-3:30</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -633,20 +625,15 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -658,27 +645,29 @@
           <t>Kate North</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>2</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -687,11 +676,6 @@
         </is>
       </c>
       <c r="H6" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -703,17 +687,19 @@
           <t>Emerson Metzger</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>2</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -732,11 +718,6 @@
         </is>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -748,12 +729,14 @@
           <t>Avery Larsen</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>2</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3:30-8</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -763,7 +746,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -777,11 +760,6 @@
         </is>
       </c>
       <c r="H8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -793,17 +771,19 @@
           <t>Austin Page</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>2</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10:30-3:30</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -813,7 +793,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -822,11 +802,6 @@
         </is>
       </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -838,12 +813,14 @@
           <t xml:space="preserve">Riley White </t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>3</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -867,11 +844,6 @@
         </is>
       </c>
       <c r="H10" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -883,8 +855,10 @@
           <t>Robert Wade</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>3</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -903,20 +877,15 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -928,12 +897,14 @@
           <t>Tatum Plunk</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>3</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10:30-3:30</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -948,20 +919,15 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -973,8 +939,10 @@
           <t>Michael Vangruber</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>3</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:30-3:30</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -988,7 +956,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1002,11 +970,6 @@
         </is>
       </c>
       <c r="H13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1018,12 +981,14 @@
           <t>Jackson Blakely</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>3</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>3:30-8</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1038,7 +1003,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1047,11 +1012,6 @@
         </is>
       </c>
       <c r="H14" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1063,27 +1023,29 @@
           <t>Addison Clark</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>3</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1092,11 +1054,6 @@
         </is>
       </c>
       <c r="H15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1108,8 +1065,10 @@
           <t>Madison Johnson</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>3</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>3:30-8</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1118,7 +1077,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1133,15 +1092,10 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1153,8 +1107,10 @@
           <t>Nathan Debergh</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>3</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>3:30-8</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1163,7 +1119,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1173,20 +1129,15 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1198,8 +1149,10 @@
           <t>Asher Bobbett</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>4</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1227,11 +1180,6 @@
         </is>
       </c>
       <c r="H18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1243,22 +1191,24 @@
           <t>Blake Ucherek</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>4</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>3:30-8</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1272,11 +1222,6 @@
         </is>
       </c>
       <c r="H19" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1288,8 +1233,10 @@
           <t>Brent Horwitz</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>4</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1317,11 +1264,6 @@
         </is>
       </c>
       <c r="H20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1333,8 +1275,10 @@
           <t xml:space="preserve">Ethan Van Horn </t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>4</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1348,25 +1292,20 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1378,8 +1317,10 @@
           <t>Kai King</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>4</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:30-3:30</t>
+        </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1388,12 +1329,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1403,15 +1344,10 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1423,17 +1359,19 @@
           <t>Madeline Ellison</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>4</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1443,20 +1381,15 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1468,40 +1401,37 @@
           <t>Tyler Carpenter</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>4</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>3:30-8</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1513,8 +1443,10 @@
           <t xml:space="preserve">Holden </t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>4</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1542,11 +1474,6 @@
         </is>
       </c>
       <c r="H25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1558,8 +1485,10 @@
           <t>Isabella</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>4</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1583,15 +1512,10 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1603,27 +1527,29 @@
           <t xml:space="preserve">Jayden Garcia </t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>4</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>10:30-3:30</t>
+        </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1632,11 +1558,6 @@
         </is>
       </c>
       <c r="H27" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1648,17 +1569,19 @@
           <t>Naya Okonkwo</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>4</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1668,20 +1591,15 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
-        <is>
-          <t>OFF</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
         <is>
           <t>X</t>
         </is>

</xml_diff>

<commit_message>
New version of guard schedule maker. The scrypt now generates the schedule with all the day adjustments. In addition, the website now allows for user registration and stores requested time off.
</commit_message>
<xml_diff>
--- a/updated_schedule.xlsx
+++ b/updated_schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Names</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Saturday </t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -521,37 +521,37 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>June18th</t>
+          <t>July2nd</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>June19th</t>
+          <t>Jully3rd</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>June20th</t>
+          <t>July4th</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>June21st</t>
+          <t>July5th</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>June22nd</t>
+          <t>July6th</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>June23rd</t>
+          <t>July7th</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>June24th</t>
+          <t>July8th</t>
         </is>
       </c>
     </row>
@@ -605,32 +605,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -647,22 +647,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:00-3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -689,17 +689,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -736,27 +736,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:00-3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:15-4</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -773,32 +773,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:00-3:30</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -815,27 +815,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:00-3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-4</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -857,12 +857,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -904,27 +904,27 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -941,32 +941,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>3:30-8</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>10:00-3:30</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>10:30-3:30</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>3:30-8</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>X</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -983,27 +983,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>1:00-6:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1025,32 +1025,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:00-3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-4</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>1:00-6:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1067,32 +1067,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-4</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:00-3:30</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:45-3:30</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1109,22 +1109,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1134,7 +1134,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1193,27 +1193,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1230,22 +1230,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Brent Horwitz</t>
+          <t xml:space="preserve">Ethan Van Horn </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1272,32 +1272,32 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ethan Van Horn </t>
+          <t>Kai King</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>11:00-5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1314,17 +1314,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Kai King</t>
+          <t>Madeline Ellison</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1334,17 +1334,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:45-3:30</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1356,7 +1356,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Madeline Ellison</t>
+          <t>Tyler Carpenter</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1371,22 +1371,22 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1398,37 +1398,37 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Tyler Carpenter</t>
+          <t xml:space="preserve">Holden </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1440,37 +1440,37 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Holden </t>
+          <t xml:space="preserve">Jayden Garcia </t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-4</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1482,37 +1482,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Isabella</t>
+          <t>Naya Okonkwo</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>3:00-7</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:45-3:30</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1524,37 +1524,37 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jayden Garcia </t>
+          <t>Bella Hamilton</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>X</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>12:00-6</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-4</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1566,7 +1566,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Naya Okonkwo</t>
+          <t>Phillip Thompson</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1576,22 +1576,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:00-3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>1:00-6:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1600,6 +1600,48 @@
         </is>
       </c>
       <c r="H28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Brent Horwitz</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>X</t>
         </is>

</xml_diff>

<commit_message>
New version of guard schedule maker. Website now allows for the deletion of requested time off and when registering requires a first and last name. Along with better style.
</commit_message>
<xml_diff>
--- a/updated_schedule.xlsx
+++ b/updated_schedule.xlsx
@@ -647,14 +647,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>10:15-3:30</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>10:15-3:30</t>
-        </is>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>10:00-3</t>
@@ -667,12 +667,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>1:00-6:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -751,12 +751,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:00-3:30</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>1:00-6:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -793,12 +793,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10:00-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -857,12 +857,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10:15-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:30-3:30</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1:00-6:00</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1025,14 +1025,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>10:15-3:30</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>10:30-3:30</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>10:30-3:30</t>
-        </is>
-      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>10:00-3</t>
@@ -1045,12 +1045,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:00-3:30</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1:00-6:00</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1067,12 +1067,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1082,17 +1082,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10:30-4</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10:00-3:30</t>
+          <t>10:15-3:30</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10:45-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4:00-9</t>
+          <t>1:00-6:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1361,12 +1361,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3:30-8</t>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1460,12 +1460,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>10:30-4</t>
+          <t>4:00-9</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>10:15-3:30</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1487,7 +1487,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:30-3:30</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4:00-9</t>
+          <t>10:30-4</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>10:45-3:30</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1:00-6:00</t>
+          <t>10:30-4</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>3:30-8</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">

</xml_diff>